<commit_message>
DAY 08 - excel automation day 2
</commit_message>
<xml_diff>
--- a/Employees.xlsx
+++ b/Employees.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekb24/IdeaProjects/CucumberProjectB24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekb24/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAD28BC-FD6C-2748-B535-5C3B8A369DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE2DFD5-AB63-8F4C-93B8-FB08278CF2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6700" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{3463B30F-B23A-1844-91CB-48DD17889895}"/>
+    <workbookView xWindow="5080" yWindow="2400" windowWidth="28040" windowHeight="17440" xr2:uid="{3463B30F-B23A-1844-91CB-48DD17889895}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -458,7 +458,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="242" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>